<commit_message>
Added new column - Email
</commit_message>
<xml_diff>
--- a/dataFiles/jobsList.xlsx
+++ b/dataFiles/jobsList.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="79">
   <si>
     <t>Sl Num</t>
   </si>
@@ -23,118 +23,232 @@
     <t>Closing Date</t>
   </si>
   <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Alzone Software (P) Ltd</t>
+  </si>
+  <si>
+    <t>25,July 2025</t>
+  </si>
+  <si>
+    <t>careers@alzonesoftware.com</t>
+  </si>
+  <si>
+    <t>Reflections Info Systems (P) Ltd</t>
+  </si>
+  <si>
+    <t>Careers@reflectionsinfos.com</t>
+  </si>
+  <si>
+    <t>TILTLABS CONSULTANCY SERVICES (P) Ltd</t>
+  </si>
+  <si>
+    <t>08,Aug 2025</t>
+  </si>
+  <si>
+    <t>careers@tiltlabs.io</t>
+  </si>
+  <si>
+    <t>RM Education Solutions India (P) Ltd</t>
+  </si>
+  <si>
+    <t>14,Aug 2025</t>
+  </si>
+  <si>
+    <t>talent@in.rm.com</t>
+  </si>
+  <si>
+    <t>REIZEND (P) Ltd</t>
+  </si>
+  <si>
+    <t>31,July 2025</t>
+  </si>
+  <si>
+    <t>careers@reizend.ai</t>
+  </si>
+  <si>
+    <t>Zybo Tech Lab (P) Ltd</t>
+  </si>
+  <si>
+    <t>jobs@zybotechlab.com</t>
+  </si>
+  <si>
+    <t>Spericorn Technology (P) Ltd</t>
+  </si>
+  <si>
+    <t>careers@spericorn.com</t>
+  </si>
+  <si>
+    <t>Faith InfoTech India (P) Ltd</t>
+  </si>
+  <si>
+    <t>hr@faithinfotech.in</t>
+  </si>
+  <si>
+    <t>Appfabs Innovation (P) Ltd</t>
+  </si>
+  <si>
+    <t>04,Aug 2025</t>
+  </si>
+  <si>
+    <t>careers@appfabs.in</t>
+  </si>
+  <si>
+    <t>06,Sept 2025</t>
+  </si>
+  <si>
+    <t>03,Aug 2025</t>
+  </si>
+  <si>
+    <t>careers@reizendretail.in</t>
+  </si>
+  <si>
+    <t>Waib3 Technologies (OPC) Pvt. Ltd</t>
+  </si>
+  <si>
+    <t>careers@waib3tech.com</t>
+  </si>
+  <si>
+    <t>TKey Education Solutions (P) Ltd [Arbor]</t>
+  </si>
+  <si>
+    <t>15,Aug 2025</t>
+  </si>
+  <si>
+    <t>hr.india@arbor-education.com</t>
+  </si>
+  <si>
+    <t>Lean Transitions Solutions</t>
+  </si>
+  <si>
+    <t>careers@ltslean.com</t>
+  </si>
+  <si>
+    <t>DIAGNAL TECHNOLOGIES (P) Ltd</t>
+  </si>
+  <si>
+    <t>28,Aug 2025</t>
+  </si>
+  <si>
+    <t>vivekkumar.jaiswal@diagnal.com</t>
+  </si>
+  <si>
     <t>Techversant Infotech (P) Ltd</t>
   </si>
   <si>
-    <t>25,July 2025</t>
-  </si>
-  <si>
-    <t>REIZEND (P) Ltd</t>
-  </si>
-  <si>
-    <t>31,July 2025</t>
-  </si>
-  <si>
-    <t>02,Sept 2025</t>
-  </si>
-  <si>
-    <t>03,Aug 2025</t>
+    <t>careers@techversantinfotech.com</t>
+  </si>
+  <si>
+    <t>KENLAND IT SOLUTIONS (P) Ltd</t>
+  </si>
+  <si>
+    <t>recruiter@kenland.in</t>
+  </si>
+  <si>
+    <t>Xminds Infotech (P) Ltd</t>
+  </si>
+  <si>
+    <t>careers@xminds.com</t>
+  </si>
+  <si>
+    <t>Kvaliteta Systems and Solutions (P) Ltd</t>
+  </si>
+  <si>
+    <t>30,July 2025</t>
+  </si>
+  <si>
+    <t>hr@kvaliteta.in</t>
+  </si>
+  <si>
+    <t>Marvelloux Apps (P) Ltd</t>
+  </si>
+  <si>
+    <t>hr@marvelloux.com</t>
+  </si>
+  <si>
+    <t>Ospyn Technologies Ltd</t>
+  </si>
+  <si>
+    <t>careers@ospyn.com</t>
+  </si>
+  <si>
+    <t>NeedStreet Web Technologies (P) Ltd</t>
+  </si>
+  <si>
+    <t>jobs@needstret.com</t>
+  </si>
+  <si>
+    <t>jobs@needstreet.com</t>
+  </si>
+  <si>
+    <t>05,Sept 2025</t>
+  </si>
+  <si>
+    <t>Zoondia Software (P) Ltd</t>
+  </si>
+  <si>
+    <t>recruit@zoondia.in</t>
+  </si>
+  <si>
+    <t>Timesworld Media and Technology Solutions (P) Ltd</t>
+  </si>
+  <si>
+    <t>hr.tvm@timesworld.com</t>
+  </si>
+  <si>
+    <t>ECESIS CARE (P) Ltd</t>
+  </si>
+  <si>
+    <t>30,Aug 2025</t>
+  </si>
+  <si>
+    <t>Amrithas@ecesistech.com</t>
+  </si>
+  <si>
+    <t>Pearlsoft Technologies LLP</t>
+  </si>
+  <si>
+    <t>11,Aug 2025</t>
+  </si>
+  <si>
+    <t>renjini.r@pearlsofttechnologies.co.in</t>
+  </si>
+  <si>
+    <t>ATEAM INFOSOFT SOLUTIONS Old</t>
+  </si>
+  <si>
+    <t>24,July 2025</t>
+  </si>
+  <si>
+    <t>recruitment@ateamsoftsolutions.com</t>
+  </si>
+  <si>
+    <t>teamhr@appfabs.in</t>
+  </si>
+  <si>
+    <t>ARS Traffic &amp; Transport Technology India (P) Ltd</t>
+  </si>
+  <si>
+    <t>31,Aug 2025</t>
+  </si>
+  <si>
+    <t>ankitac@arstraffic.com</t>
+  </si>
+  <si>
+    <t>01,Aug 2025</t>
   </si>
   <si>
     <t>Softnotions Technologies (P) Ltd</t>
   </si>
   <si>
-    <t>22,July 2025</t>
-  </si>
-  <si>
-    <t>Alzone Software (P) Ltd</t>
-  </si>
-  <si>
-    <t>Appfabs Innovation (P) Ltd</t>
-  </si>
-  <si>
-    <t>04,Aug 2025</t>
-  </si>
-  <si>
-    <t>Reflections Info Systems (P) Ltd</t>
-  </si>
-  <si>
-    <t>Ospyn Technologies Ltd</t>
-  </si>
-  <si>
-    <t>NeedStreet Web Technologies (P) Ltd</t>
-  </si>
-  <si>
-    <t>ECESIS CARE (P) Ltd</t>
-  </si>
-  <si>
-    <t>30,Aug 2025</t>
-  </si>
-  <si>
-    <t>TKey Education Solutions (P) Ltd [Arbor]</t>
-  </si>
-  <si>
-    <t>15,Aug 2025</t>
+    <t>recruitment@softnotions.com</t>
+  </si>
+  <si>
+    <t>recruitment@ecesistech.com</t>
   </si>
   <si>
     <t>23,Aug 2025</t>
-  </si>
-  <si>
-    <t>ATEAM INFOSOFT SOLUTIONS Old</t>
-  </si>
-  <si>
-    <t>24,July 2025</t>
-  </si>
-  <si>
-    <t>Zybo Tech Lab (P) Ltd</t>
-  </si>
-  <si>
-    <t>KENLAND IT SOLUTIONS (P) Ltd</t>
-  </si>
-  <si>
-    <t>Xminds Infotech (P) Ltd</t>
-  </si>
-  <si>
-    <t>05,Sept 2025</t>
-  </si>
-  <si>
-    <t>01,Aug 2025</t>
-  </si>
-  <si>
-    <t>Timesworld Media and Technology Solutions (P) Ltd</t>
-  </si>
-  <si>
-    <t>Spericorn Technology (P) Ltd</t>
-  </si>
-  <si>
-    <t>RM Education Solutions India (P) Ltd</t>
-  </si>
-  <si>
-    <t>14,Aug 2025</t>
-  </si>
-  <si>
-    <t>Marvelloux Apps (P) Ltd</t>
-  </si>
-  <si>
-    <t>30,July 2025</t>
-  </si>
-  <si>
-    <t>Pearlsoft Technologies LLP</t>
-  </si>
-  <si>
-    <t>11,Aug 2025</t>
-  </si>
-  <si>
-    <t>Zoondia Software (P) Ltd</t>
-  </si>
-  <si>
-    <t>DIAGNAL TECHNOLOGIES (P) Ltd</t>
-  </si>
-  <si>
-    <t>28,Aug 2025</t>
-  </si>
-  <si>
-    <t>Faith InfoTech India (P) Ltd</t>
   </si>
 </sst>
 </file>
@@ -179,7 +293,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C54"/>
+  <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -195,16 +309,22 @@
       <c r="C1" t="s" s="0">
         <v>2</v>
       </c>
+      <c r="D1" t="s" s="0">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n" s="0">
         <v>1.0</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D2" t="s" s="0">
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -212,10 +332,13 @@
         <v>2.0</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="D3" t="s" s="0">
+        <v>8</v>
       </c>
     </row>
     <row r="4">
@@ -223,10 +346,13 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>6</v>
+        <v>10</v>
+      </c>
+      <c r="D4" t="s" s="0">
+        <v>11</v>
       </c>
     </row>
     <row r="5">
@@ -234,10 +360,13 @@
         <v>4.0</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s" s="0">
-        <v>7</v>
+        <v>13</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>14</v>
       </c>
     </row>
     <row r="6">
@@ -245,10 +374,13 @@
         <v>5.0</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="7">
@@ -256,10 +388,13 @@
         <v>6.0</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>10</v>
+        <v>5</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>19</v>
       </c>
     </row>
     <row r="8">
@@ -267,10 +402,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>21</v>
       </c>
     </row>
     <row r="9">
@@ -278,10 +416,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>23</v>
       </c>
     </row>
     <row r="10">
@@ -289,10 +430,13 @@
         <v>9.0</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>13</v>
+        <v>25</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>26</v>
       </c>
     </row>
     <row r="11">
@@ -300,10 +444,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>4</v>
+        <v>27</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="12">
@@ -311,10 +458,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>8</v>
       </c>
     </row>
     <row r="13">
@@ -325,7 +475,10 @@
         <v>15</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>4</v>
+        <v>28</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>29</v>
       </c>
     </row>
     <row r="14">
@@ -333,10 +486,13 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>31</v>
       </c>
     </row>
     <row r="15">
@@ -344,10 +500,13 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>18</v>
+        <v>33</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>34</v>
       </c>
     </row>
     <row r="16">
@@ -355,10 +514,13 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s" s="0">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>36</v>
       </c>
     </row>
     <row r="17">
@@ -366,10 +528,13 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>5</v>
+        <v>35</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>21</v>
+        <v>5</v>
+      </c>
+      <c r="D17" t="s" s="0">
+        <v>36</v>
       </c>
     </row>
     <row r="18">
@@ -377,10 +542,13 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C18" t="s" s="0">
-        <v>23</v>
+        <v>38</v>
+      </c>
+      <c r="D18" t="s" s="0">
+        <v>39</v>
       </c>
     </row>
     <row r="19">
@@ -388,10 +556,13 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="D19" t="s" s="0">
+        <v>41</v>
       </c>
     </row>
     <row r="20">
@@ -399,10 +570,13 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>3</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>6</v>
+        <v>33</v>
+      </c>
+      <c r="D20" t="s" s="0">
+        <v>43</v>
       </c>
     </row>
     <row r="21">
@@ -410,10 +584,13 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="s" s="0">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s" s="0">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D21" t="s" s="0">
+        <v>41</v>
       </c>
     </row>
     <row r="22">
@@ -421,10 +598,13 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>20</v>
+        <v>27</v>
+      </c>
+      <c r="D22" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="23">
@@ -432,10 +612,13 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D23" t="s" s="0">
+        <v>45</v>
       </c>
     </row>
     <row r="24">
@@ -443,10 +626,13 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>4</v>
+        <v>47</v>
+      </c>
+      <c r="D24" t="s" s="0">
+        <v>48</v>
       </c>
     </row>
     <row r="25">
@@ -454,10 +640,13 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>8</v>
+        <v>16</v>
+      </c>
+      <c r="D25" t="s" s="0">
+        <v>50</v>
       </c>
     </row>
     <row r="26">
@@ -465,10 +654,13 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>12</v>
+        <v>51</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>13</v>
+        <v>5</v>
+      </c>
+      <c r="D26" t="s" s="0">
+        <v>52</v>
       </c>
     </row>
     <row r="27">
@@ -476,10 +668,13 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>27</v>
+        <v>5</v>
+      </c>
+      <c r="D27" t="s" s="0">
+        <v>8</v>
       </c>
     </row>
     <row r="28">
@@ -487,10 +682,13 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>3</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>4</v>
+        <v>33</v>
+      </c>
+      <c r="D28" t="s" s="0">
+        <v>34</v>
       </c>
     </row>
     <row r="29">
@@ -498,10 +696,13 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>14</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="D29" t="s" s="0">
+        <v>54</v>
       </c>
     </row>
     <row r="30">
@@ -509,10 +710,13 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>17</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s" s="0">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="D30" t="s" s="0">
+        <v>55</v>
       </c>
     </row>
     <row r="31">
@@ -520,10 +724,13 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>6</v>
+        <v>56</v>
+      </c>
+      <c r="D31" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="32">
@@ -531,10 +738,13 @@
         <v>31.0</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>8</v>
+        <v>5</v>
+      </c>
+      <c r="D32" t="s" s="0">
+        <v>41</v>
       </c>
     </row>
     <row r="33">
@@ -542,10 +752,13 @@
         <v>32.0</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>22</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>28</v>
+        <v>47</v>
+      </c>
+      <c r="D33" t="s" s="0">
+        <v>58</v>
       </c>
     </row>
     <row r="34">
@@ -553,10 +766,13 @@
         <v>33.0</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>4</v>
+        <v>28</v>
+      </c>
+      <c r="D34" t="s" s="0">
+        <v>29</v>
       </c>
     </row>
     <row r="35">
@@ -564,10 +780,13 @@
         <v>34.0</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>17</v>
+        <v>59</v>
       </c>
       <c r="C35" t="s" s="0">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="D35" t="s" s="0">
+        <v>60</v>
       </c>
     </row>
     <row r="36">
@@ -575,10 +794,13 @@
         <v>35.0</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>24</v>
+        <v>61</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>4</v>
+        <v>62</v>
+      </c>
+      <c r="D36" t="s" s="0">
+        <v>63</v>
       </c>
     </row>
     <row r="37">
@@ -586,10 +808,13 @@
         <v>36.0</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>6</v>
+        <v>16</v>
+      </c>
+      <c r="D37" t="s" s="0">
+        <v>21</v>
       </c>
     </row>
     <row r="38">
@@ -597,10 +822,13 @@
         <v>37.0</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C38" t="s" s="0">
-        <v>6</v>
+        <v>25</v>
+      </c>
+      <c r="D38" t="s" s="0">
+        <v>26</v>
       </c>
     </row>
     <row r="39">
@@ -608,10 +836,13 @@
         <v>38.0</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>13</v>
+        <v>56</v>
+      </c>
+      <c r="D39" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="40">
@@ -619,10 +850,13 @@
         <v>39.0</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>20</v>
+        <v>5</v>
+      </c>
+      <c r="D40" t="s" s="0">
+        <v>52</v>
       </c>
     </row>
     <row r="41">
@@ -630,10 +864,13 @@
         <v>40.0</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="D41" t="s" s="0">
+        <v>29</v>
       </c>
     </row>
     <row r="42">
@@ -641,10 +878,13 @@
         <v>41.0</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="D42" t="s" s="0">
+        <v>19</v>
       </c>
     </row>
     <row r="43">
@@ -652,10 +892,13 @@
         <v>42.0</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="D43" t="s" s="0">
+        <v>41</v>
       </c>
     </row>
     <row r="44">
@@ -663,10 +906,13 @@
         <v>43.0</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>33</v>
+        <v>15</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>6</v>
+        <v>28</v>
+      </c>
+      <c r="D44" t="s" s="0">
+        <v>29</v>
       </c>
     </row>
     <row r="45">
@@ -674,10 +920,13 @@
         <v>44.0</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>5</v>
+        <v>64</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>6</v>
+        <v>65</v>
+      </c>
+      <c r="D45" t="s" s="0">
+        <v>66</v>
       </c>
     </row>
     <row r="46">
@@ -685,10 +934,13 @@
         <v>45.0</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>34</v>
+        <v>16</v>
+      </c>
+      <c r="D46" t="s" s="0">
+        <v>41</v>
       </c>
     </row>
     <row r="47">
@@ -696,10 +948,13 @@
         <v>46.0</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="C47" t="s" s="0">
-        <v>36</v>
+        <v>68</v>
+      </c>
+      <c r="D47" t="s" s="0">
+        <v>69</v>
       </c>
     </row>
     <row r="48">
@@ -707,10 +962,13 @@
         <v>47.0</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>6</v>
+        <v>56</v>
+      </c>
+      <c r="D48" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="49">
@@ -718,10 +976,13 @@
         <v>48.0</v>
       </c>
       <c r="B49" t="s" s="0">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="C49" t="s" s="0">
-        <v>27</v>
+        <v>16</v>
+      </c>
+      <c r="D49" t="s" s="0">
+        <v>17</v>
       </c>
     </row>
     <row r="50">
@@ -729,10 +990,13 @@
         <v>49.0</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>6</v>
+        <v>25</v>
+      </c>
+      <c r="D50" t="s" s="0">
+        <v>70</v>
       </c>
     </row>
     <row r="51">
@@ -740,10 +1004,13 @@
         <v>50.0</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>34</v>
+        <v>72</v>
+      </c>
+      <c r="D51" t="s" s="0">
+        <v>73</v>
       </c>
     </row>
     <row r="52">
@@ -751,10 +1018,13 @@
         <v>51.0</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>39</v>
+        <v>74</v>
+      </c>
+      <c r="D52" t="s" s="0">
+        <v>69</v>
       </c>
     </row>
     <row r="53">
@@ -762,10 +1032,13 @@
         <v>52.0</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>6</v>
+        <v>47</v>
+      </c>
+      <c r="D53" t="s" s="0">
+        <v>76</v>
       </c>
     </row>
     <row r="54">
@@ -773,10 +1046,195 @@
         <v>53.0</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>6</v>
+        <v>27</v>
+      </c>
+      <c r="D54" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n" s="0">
+        <v>54.0</v>
+      </c>
+      <c r="B55" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C55" t="s" s="0">
+        <v>62</v>
+      </c>
+      <c r="D55" t="s" s="0">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n" s="0">
+        <v>55.0</v>
+      </c>
+      <c r="B56" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="C56" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D56" t="s" s="0">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n" s="0">
+        <v>56.0</v>
+      </c>
+      <c r="B57" t="s" s="0">
+        <v>59</v>
+      </c>
+      <c r="C57" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D57" t="s" s="0">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n" s="0">
+        <v>57.0</v>
+      </c>
+      <c r="B58" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C58" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D58" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n" s="0">
+        <v>58.0</v>
+      </c>
+      <c r="B59" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C59" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="D59" t="s" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n" s="0">
+        <v>59.0</v>
+      </c>
+      <c r="B60" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="C60" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D60" t="s" s="0">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="n" s="0">
+        <v>60.0</v>
+      </c>
+      <c r="B61" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C61" t="s" s="0">
+        <v>47</v>
+      </c>
+      <c r="D61" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="n" s="0">
+        <v>61.0</v>
+      </c>
+      <c r="B62" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C62" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D62" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="n" s="0">
+        <v>62.0</v>
+      </c>
+      <c r="B63" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C63" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D63" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="n" s="0">
+        <v>63.0</v>
+      </c>
+      <c r="B64" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C64" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="D64" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="n" s="0">
+        <v>64.0</v>
+      </c>
+      <c r="B65" t="s" s="0">
+        <v>40</v>
+      </c>
+      <c r="C65" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D65" t="s" s="0">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="n" s="0">
+        <v>65.0</v>
+      </c>
+      <c r="B66" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="C66" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D66" t="s" s="0">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="n" s="0">
+        <v>66.0</v>
+      </c>
+      <c r="B67" t="s" s="0">
+        <v>51</v>
+      </c>
+      <c r="C67" t="s" s="0">
+        <v>16</v>
+      </c>
+      <c r="D67" t="s" s="0">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
made execution in headless mode
</commit_message>
<xml_diff>
--- a/dataFiles/jobsList.xlsx
+++ b/dataFiles/jobsList.xlsx
@@ -26,19 +26,196 @@
     <t>Email</t>
   </si>
   <si>
+    <t>Pearlsoft Technologies LLP</t>
+  </si>
+  <si>
+    <t>11,Aug 2025</t>
+  </si>
+  <si>
+    <t>renjini.r@pearlsofttechnologies.co.in</t>
+  </si>
+  <si>
+    <t>Softnotions Technologies (P) Ltd</t>
+  </si>
+  <si>
+    <t>30,July 2025</t>
+  </si>
+  <si>
+    <t>recruitment@softnotions.com</t>
+  </si>
+  <si>
+    <t>Techversant Infotech (P) Ltd</t>
+  </si>
+  <si>
+    <t>careers@techversantinfotech.com</t>
+  </si>
+  <si>
+    <t>ATEAM INFOSOFT SOLUTIONS Old</t>
+  </si>
+  <si>
+    <t>01,Aug 2025</t>
+  </si>
+  <si>
+    <t>recruitment@ateamsoftsolutions.com</t>
+  </si>
+  <si>
+    <t>NeedStreet Web Technologies (P) Ltd</t>
+  </si>
+  <si>
+    <t>31,July 2025</t>
+  </si>
+  <si>
+    <t>jobs@needstreet.com</t>
+  </si>
+  <si>
+    <t>REIZEND (P) Ltd</t>
+  </si>
+  <si>
+    <t>05,Sept 2025</t>
+  </si>
+  <si>
+    <t>careers@reizend.ai</t>
+  </si>
+  <si>
+    <t>Appfabs Innovation (P) Ltd</t>
+  </si>
+  <si>
+    <t>04,Aug 2025</t>
+  </si>
+  <si>
+    <t>careers@appfabs.in</t>
+  </si>
+  <si>
+    <t>TKey Education Solutions (P) Ltd [Arbor]</t>
+  </si>
+  <si>
+    <t>15,Aug 2025</t>
+  </si>
+  <si>
+    <t>hr.india@arbor-education.com</t>
+  </si>
+  <si>
+    <t>Spericorn Technology (P) Ltd</t>
+  </si>
+  <si>
+    <t>careers@spericorn.com</t>
+  </si>
+  <si>
+    <t>Ospyn Technologies Ltd</t>
+  </si>
+  <si>
+    <t>careers@ospyn.com</t>
+  </si>
+  <si>
+    <t>Reflections Info Systems (P) Ltd</t>
+  </si>
+  <si>
+    <t>25,July 2025</t>
+  </si>
+  <si>
+    <t>Careers@reflectionsinfos.com</t>
+  </si>
+  <si>
+    <t>KENLAND IT SOLUTIONS (P) Ltd</t>
+  </si>
+  <si>
+    <t>recruiter@kenland.in</t>
+  </si>
+  <si>
+    <t>Zybo Tech Lab (P) Ltd</t>
+  </si>
+  <si>
+    <t>jobs@zybotechlab.com</t>
+  </si>
+  <si>
+    <t>Zoondia Software (P) Ltd</t>
+  </si>
+  <si>
+    <t>recruit@zoondia.in</t>
+  </si>
+  <si>
+    <t>06,Sept 2025</t>
+  </si>
+  <si>
+    <t>DIAGNAL TECHNOLOGIES (P) Ltd</t>
+  </si>
+  <si>
+    <t>28,Aug 2025</t>
+  </si>
+  <si>
+    <t>vivekkumar.jaiswal@diagnal.com</t>
+  </si>
+  <si>
+    <t>03,Aug 2025</t>
+  </si>
+  <si>
+    <t>careers@reizendretail.in</t>
+  </si>
+  <si>
+    <t>RM Education Solutions India (P) Ltd</t>
+  </si>
+  <si>
+    <t>14,Aug 2025</t>
+  </si>
+  <si>
+    <t>talent@in.rm.com</t>
+  </si>
+  <si>
+    <t>Waib3 Technologies (OPC) Pvt. Ltd</t>
+  </si>
+  <si>
+    <t>careers@waib3tech.com</t>
+  </si>
+  <si>
+    <t>Lean Transitions Solutions</t>
+  </si>
+  <si>
+    <t>careers@ltslean.com</t>
+  </si>
+  <si>
+    <t>24,July 2025</t>
+  </si>
+  <si>
+    <t>teamhr@appfabs.in</t>
+  </si>
+  <si>
+    <t>23,Aug 2025</t>
+  </si>
+  <si>
+    <t>Marvelloux Apps (P) Ltd</t>
+  </si>
+  <si>
+    <t>hr@marvelloux.com</t>
+  </si>
+  <si>
+    <t>Kvaliteta Systems and Solutions (P) Ltd</t>
+  </si>
+  <si>
+    <t>hr@kvaliteta.in</t>
+  </si>
+  <si>
+    <t>Timesworld Media and Technology Solutions (P) Ltd</t>
+  </si>
+  <si>
+    <t>hr.tvm@timesworld.com</t>
+  </si>
+  <si>
+    <t>ECESIS CARE (P) Ltd</t>
+  </si>
+  <si>
+    <t>30,Aug 2025</t>
+  </si>
+  <si>
+    <t>Amrithas@ecesistech.com</t>
+  </si>
+  <si>
     <t>Alzone Software (P) Ltd</t>
   </si>
   <si>
-    <t>25,July 2025</t>
-  </si>
-  <si>
     <t>careers@alzonesoftware.com</t>
   </si>
   <si>
-    <t>Reflections Info Systems (P) Ltd</t>
-  </si>
-  <si>
-    <t>Careers@reflectionsinfos.com</t>
+    <t>jobs@needstret.com</t>
   </si>
   <si>
     <t>TILTLABS CONSULTANCY SERVICES (P) Ltd</t>
@@ -50,183 +227,18 @@
     <t>careers@tiltlabs.io</t>
   </si>
   <si>
-    <t>RM Education Solutions India (P) Ltd</t>
-  </si>
-  <si>
-    <t>14,Aug 2025</t>
-  </si>
-  <si>
-    <t>talent@in.rm.com</t>
-  </si>
-  <si>
-    <t>REIZEND (P) Ltd</t>
-  </si>
-  <si>
-    <t>31,July 2025</t>
-  </si>
-  <si>
-    <t>careers@reizend.ai</t>
-  </si>
-  <si>
-    <t>Zybo Tech Lab (P) Ltd</t>
-  </si>
-  <si>
-    <t>jobs@zybotechlab.com</t>
-  </si>
-  <si>
-    <t>Spericorn Technology (P) Ltd</t>
-  </si>
-  <si>
-    <t>careers@spericorn.com</t>
-  </si>
-  <si>
     <t>Faith InfoTech India (P) Ltd</t>
   </si>
   <si>
     <t>hr@faithinfotech.in</t>
   </si>
   <si>
-    <t>Appfabs Innovation (P) Ltd</t>
-  </si>
-  <si>
-    <t>04,Aug 2025</t>
-  </si>
-  <si>
-    <t>careers@appfabs.in</t>
-  </si>
-  <si>
-    <t>06,Sept 2025</t>
-  </si>
-  <si>
-    <t>03,Aug 2025</t>
-  </si>
-  <si>
-    <t>careers@reizendretail.in</t>
-  </si>
-  <si>
-    <t>Waib3 Technologies (OPC) Pvt. Ltd</t>
-  </si>
-  <si>
-    <t>careers@waib3tech.com</t>
-  </si>
-  <si>
-    <t>TKey Education Solutions (P) Ltd [Arbor]</t>
-  </si>
-  <si>
-    <t>15,Aug 2025</t>
-  </si>
-  <si>
-    <t>hr.india@arbor-education.com</t>
-  </si>
-  <si>
-    <t>Lean Transitions Solutions</t>
-  </si>
-  <si>
-    <t>careers@ltslean.com</t>
-  </si>
-  <si>
-    <t>DIAGNAL TECHNOLOGIES (P) Ltd</t>
-  </si>
-  <si>
-    <t>28,Aug 2025</t>
-  </si>
-  <si>
-    <t>vivekkumar.jaiswal@diagnal.com</t>
-  </si>
-  <si>
-    <t>Techversant Infotech (P) Ltd</t>
-  </si>
-  <si>
-    <t>careers@techversantinfotech.com</t>
-  </si>
-  <si>
-    <t>KENLAND IT SOLUTIONS (P) Ltd</t>
-  </si>
-  <si>
-    <t>recruiter@kenland.in</t>
-  </si>
-  <si>
     <t>Xminds Infotech (P) Ltd</t>
   </si>
   <si>
     <t>careers@xminds.com</t>
   </si>
   <si>
-    <t>Kvaliteta Systems and Solutions (P) Ltd</t>
-  </si>
-  <si>
-    <t>30,July 2025</t>
-  </si>
-  <si>
-    <t>hr@kvaliteta.in</t>
-  </si>
-  <si>
-    <t>Marvelloux Apps (P) Ltd</t>
-  </si>
-  <si>
-    <t>hr@marvelloux.com</t>
-  </si>
-  <si>
-    <t>Ospyn Technologies Ltd</t>
-  </si>
-  <si>
-    <t>careers@ospyn.com</t>
-  </si>
-  <si>
-    <t>NeedStreet Web Technologies (P) Ltd</t>
-  </si>
-  <si>
-    <t>jobs@needstret.com</t>
-  </si>
-  <si>
-    <t>jobs@needstreet.com</t>
-  </si>
-  <si>
-    <t>05,Sept 2025</t>
-  </si>
-  <si>
-    <t>Zoondia Software (P) Ltd</t>
-  </si>
-  <si>
-    <t>recruit@zoondia.in</t>
-  </si>
-  <si>
-    <t>Timesworld Media and Technology Solutions (P) Ltd</t>
-  </si>
-  <si>
-    <t>hr.tvm@timesworld.com</t>
-  </si>
-  <si>
-    <t>ECESIS CARE (P) Ltd</t>
-  </si>
-  <si>
-    <t>30,Aug 2025</t>
-  </si>
-  <si>
-    <t>Amrithas@ecesistech.com</t>
-  </si>
-  <si>
-    <t>Pearlsoft Technologies LLP</t>
-  </si>
-  <si>
-    <t>11,Aug 2025</t>
-  </si>
-  <si>
-    <t>renjini.r@pearlsofttechnologies.co.in</t>
-  </si>
-  <si>
-    <t>ATEAM INFOSOFT SOLUTIONS Old</t>
-  </si>
-  <si>
-    <t>24,July 2025</t>
-  </si>
-  <si>
-    <t>recruitment@ateamsoftsolutions.com</t>
-  </si>
-  <si>
-    <t>teamhr@appfabs.in</t>
-  </si>
-  <si>
     <t>ARS Traffic &amp; Transport Technology India (P) Ltd</t>
   </si>
   <si>
@@ -236,19 +248,7 @@
     <t>ankitac@arstraffic.com</t>
   </si>
   <si>
-    <t>01,Aug 2025</t>
-  </si>
-  <si>
-    <t>Softnotions Technologies (P) Ltd</t>
-  </si>
-  <si>
-    <t>recruitment@softnotions.com</t>
-  </si>
-  <si>
     <t>recruitment@ecesistech.com</t>
-  </si>
-  <si>
-    <t>23,Aug 2025</t>
   </si>
 </sst>
 </file>
@@ -335,10 +335,10 @@
         <v>7</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4">
@@ -346,10 +346,10 @@
         <v>3.0</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s" s="0">
         <v>11</v>
@@ -391,10 +391,10 @@
         <v>18</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D7" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -402,13 +402,13 @@
         <v>7.0</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s" s="0">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9">
@@ -416,13 +416,13 @@
         <v>8.0</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="D9" t="s" s="0">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10">
@@ -444,13 +444,13 @@
         <v>10.0</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D11" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
@@ -458,13 +458,13 @@
         <v>11.0</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="C12" t="s" s="0">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D12" t="s" s="0">
-        <v>8</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13">
@@ -472,13 +472,13 @@
         <v>12.0</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C13" t="s" s="0">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s" s="0">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14">
@@ -486,13 +486,13 @@
         <v>13.0</v>
       </c>
       <c r="B14" t="s" s="0">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s" s="0">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D14" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15">
@@ -500,13 +500,13 @@
         <v>14.0</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C15" t="s" s="0">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="D15" t="s" s="0">
-        <v>34</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
@@ -514,13 +514,13 @@
         <v>15.0</v>
       </c>
       <c r="B16" t="s" s="0">
+        <v>34</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s" s="0">
         <v>35</v>
-      </c>
-      <c r="C16" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s" s="0">
-        <v>36</v>
       </c>
     </row>
     <row r="17">
@@ -528,13 +528,13 @@
         <v>16.0</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s" s="0">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D17" t="s" s="0">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18">
@@ -542,13 +542,13 @@
         <v>17.0</v>
       </c>
       <c r="B18" t="s" s="0">
+        <v>36</v>
+      </c>
+      <c r="C18" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s" s="0">
         <v>37</v>
-      </c>
-      <c r="C18" t="s" s="0">
-        <v>38</v>
-      </c>
-      <c r="D18" t="s" s="0">
-        <v>39</v>
       </c>
     </row>
     <row r="19">
@@ -556,13 +556,13 @@
         <v>18.0</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" t="s" s="0">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D19" t="s" s="0">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20">
@@ -570,13 +570,13 @@
         <v>19.0</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s" s="0">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s" s="0">
-        <v>43</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21">
@@ -584,13 +584,13 @@
         <v>20.0</v>
       </c>
       <c r="B21" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C21" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="C21" t="s" s="0">
-        <v>5</v>
-      </c>
       <c r="D21" t="s" s="0">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22">
@@ -598,13 +598,13 @@
         <v>21.0</v>
       </c>
       <c r="B22" t="s" s="0">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s" s="0">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="D22" t="s" s="0">
-        <v>17</v>
+        <v>43</v>
       </c>
     </row>
     <row r="23">
@@ -612,13 +612,13 @@
         <v>22.0</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>44</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s" s="0">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D23" t="s" s="0">
-        <v>45</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24">
@@ -626,13 +626,13 @@
         <v>23.0</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="C24" t="s" s="0">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D24" t="s" s="0">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25">
@@ -640,13 +640,13 @@
         <v>24.0</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C25" t="s" s="0">
-        <v>16</v>
+        <v>47</v>
       </c>
       <c r="D25" t="s" s="0">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26">
@@ -654,13 +654,13 @@
         <v>25.0</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>51</v>
+        <v>10</v>
       </c>
       <c r="C26" t="s" s="0">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D26" t="s" s="0">
-        <v>52</v>
+        <v>11</v>
       </c>
     </row>
     <row r="27">
@@ -668,13 +668,13 @@
         <v>26.0</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>7</v>
+        <v>49</v>
       </c>
       <c r="C27" t="s" s="0">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="D27" t="s" s="0">
-        <v>8</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28">
@@ -682,13 +682,13 @@
         <v>27.0</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="C28" t="s" s="0">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="D28" t="s" s="0">
-        <v>34</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29">
@@ -696,13 +696,13 @@
         <v>28.0</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C29" t="s" s="0">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D29" t="s" s="0">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="30">
@@ -710,13 +710,13 @@
         <v>29.0</v>
       </c>
       <c r="B30" t="s" s="0">
+        <v>12</v>
+      </c>
+      <c r="C30" t="s" s="0">
         <v>53</v>
       </c>
-      <c r="C30" t="s" s="0">
-        <v>16</v>
-      </c>
       <c r="D30" t="s" s="0">
-        <v>55</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31">
@@ -724,13 +724,13 @@
         <v>30.0</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C31" t="s" s="0">
-        <v>56</v>
+        <v>16</v>
       </c>
       <c r="D31" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="32">
@@ -738,13 +738,13 @@
         <v>31.0</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="C32" t="s" s="0">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="D32" t="s" s="0">
-        <v>41</v>
+        <v>54</v>
       </c>
     </row>
     <row r="33">
@@ -752,13 +752,13 @@
         <v>32.0</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>57</v>
+        <v>10</v>
       </c>
       <c r="C33" t="s" s="0">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D33" t="s" s="0">
-        <v>58</v>
+        <v>11</v>
       </c>
     </row>
     <row r="34">
@@ -766,13 +766,13 @@
         <v>33.0</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C34" t="s" s="0">
-        <v>28</v>
+        <v>55</v>
       </c>
       <c r="D34" t="s" s="0">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="35">
@@ -780,13 +780,13 @@
         <v>34.0</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C35" t="s" s="0">
         <v>16</v>
       </c>
       <c r="D35" t="s" s="0">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="36">
@@ -794,13 +794,13 @@
         <v>35.0</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="C36" t="s" s="0">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="D36" t="s" s="0">
-        <v>63</v>
+        <v>50</v>
       </c>
     </row>
     <row r="37">
@@ -808,13 +808,13 @@
         <v>36.0</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C37" t="s" s="0">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D37" t="s" s="0">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="38">
@@ -822,13 +822,13 @@
         <v>37.0</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C38" t="s" s="0">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D38" t="s" s="0">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39">
@@ -836,13 +836,13 @@
         <v>38.0</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="C39" t="s" s="0">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="D39" t="s" s="0">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="40">
@@ -850,13 +850,13 @@
         <v>39.0</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="C40" t="s" s="0">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="D40" t="s" s="0">
-        <v>52</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41">
@@ -864,13 +864,13 @@
         <v>40.0</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>15</v>
+        <v>31</v>
       </c>
       <c r="C41" t="s" s="0">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D41" t="s" s="0">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="42">
@@ -878,13 +878,13 @@
         <v>41.0</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s" s="0">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D42" t="s" s="0">
-        <v>19</v>
+        <v>30</v>
       </c>
     </row>
     <row r="43">
@@ -892,13 +892,13 @@
         <v>42.0</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C43" t="s" s="0">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D43" t="s" s="0">
-        <v>41</v>
+        <v>61</v>
       </c>
     </row>
     <row r="44">
@@ -906,13 +906,13 @@
         <v>43.0</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C44" t="s" s="0">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D44" t="s" s="0">
-        <v>29</v>
+        <v>45</v>
       </c>
     </row>
     <row r="45">
@@ -920,13 +920,13 @@
         <v>44.0</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="C45" t="s" s="0">
-        <v>65</v>
+        <v>32</v>
       </c>
       <c r="D45" t="s" s="0">
-        <v>66</v>
+        <v>33</v>
       </c>
     </row>
     <row r="46">
@@ -934,13 +934,13 @@
         <v>45.0</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C46" t="s" s="0">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="D46" t="s" s="0">
-        <v>41</v>
+        <v>64</v>
       </c>
     </row>
     <row r="47">
@@ -948,13 +948,13 @@
         <v>46.0</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>67</v>
+        <v>18</v>
       </c>
       <c r="C47" t="s" s="0">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="D47" t="s" s="0">
-        <v>69</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48">
@@ -962,13 +962,13 @@
         <v>47.0</v>
       </c>
       <c r="B48" t="s" s="0">
-        <v>15</v>
+        <v>65</v>
       </c>
       <c r="C48" t="s" s="0">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="D48" t="s" s="0">
-        <v>17</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49">
@@ -982,7 +982,7 @@
         <v>16</v>
       </c>
       <c r="D49" t="s" s="0">
-        <v>17</v>
+        <v>67</v>
       </c>
     </row>
     <row r="50">
@@ -990,10 +990,10 @@
         <v>49.0</v>
       </c>
       <c r="B50" t="s" s="0">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C50" t="s" s="0">
-        <v>25</v>
+        <v>69</v>
       </c>
       <c r="D50" t="s" s="0">
         <v>70</v>
@@ -1004,13 +1004,13 @@
         <v>50.0</v>
       </c>
       <c r="B51" t="s" s="0">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C51" t="s" s="0">
-        <v>72</v>
+        <v>16</v>
       </c>
       <c r="D51" t="s" s="0">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="52">
@@ -1018,13 +1018,13 @@
         <v>51.0</v>
       </c>
       <c r="B52" t="s" s="0">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C52" t="s" s="0">
-        <v>74</v>
+        <v>16</v>
       </c>
       <c r="D52" t="s" s="0">
-        <v>69</v>
+        <v>72</v>
       </c>
     </row>
     <row r="53">
@@ -1032,13 +1032,13 @@
         <v>52.0</v>
       </c>
       <c r="B53" t="s" s="0">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C53" t="s" s="0">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D53" t="s" s="0">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54">
@@ -1046,13 +1046,13 @@
         <v>53.0</v>
       </c>
       <c r="B54" t="s" s="0">
-        <v>15</v>
+        <v>51</v>
       </c>
       <c r="C54" t="s" s="0">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D54" t="s" s="0">
-        <v>17</v>
+        <v>52</v>
       </c>
     </row>
     <row r="55">
@@ -1060,13 +1060,13 @@
         <v>54.0</v>
       </c>
       <c r="B55" t="s" s="0">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="C55" t="s" s="0">
-        <v>62</v>
+        <v>16</v>
       </c>
       <c r="D55" t="s" s="0">
-        <v>63</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56">
@@ -1074,13 +1074,13 @@
         <v>55.0</v>
       </c>
       <c r="B56" t="s" s="0">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="C56" t="s" s="0">
-        <v>13</v>
+        <v>76</v>
       </c>
       <c r="D56" t="s" s="0">
-        <v>31</v>
+        <v>77</v>
       </c>
     </row>
     <row r="57">
@@ -1088,13 +1088,13 @@
         <v>56.0</v>
       </c>
       <c r="B57" t="s" s="0">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="C57" t="s" s="0">
         <v>16</v>
       </c>
       <c r="D57" t="s" s="0">
-        <v>60</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58">
@@ -1102,13 +1102,13 @@
         <v>57.0</v>
       </c>
       <c r="B58" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C58" t="s" s="0">
         <v>40</v>
       </c>
-      <c r="C58" t="s" s="0">
-        <v>16</v>
-      </c>
       <c r="D58" t="s" s="0">
-        <v>41</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59">
@@ -1116,13 +1116,13 @@
         <v>58.0</v>
       </c>
       <c r="B59" t="s" s="0">
-        <v>7</v>
+        <v>62</v>
       </c>
       <c r="C59" t="s" s="0">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="D59" t="s" s="0">
-        <v>8</v>
+        <v>78</v>
       </c>
     </row>
     <row r="60">
@@ -1130,13 +1130,13 @@
         <v>59.0</v>
       </c>
       <c r="B60" t="s" s="0">
-        <v>61</v>
+        <v>18</v>
       </c>
       <c r="C60" t="s" s="0">
-        <v>16</v>
+        <v>40</v>
       </c>
       <c r="D60" t="s" s="0">
-        <v>77</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61">
@@ -1144,13 +1144,13 @@
         <v>60.0</v>
       </c>
       <c r="B61" t="s" s="0">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="C61" t="s" s="0">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="D61" t="s" s="0">
-        <v>41</v>
+        <v>11</v>
       </c>
     </row>
     <row r="62">
@@ -1158,13 +1158,13 @@
         <v>61.0</v>
       </c>
       <c r="B62" t="s" s="0">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C62" t="s" s="0">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D62" t="s" s="0">
-        <v>17</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63">
@@ -1172,13 +1172,13 @@
         <v>62.0</v>
       </c>
       <c r="B63" t="s" s="0">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="C63" t="s" s="0">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D63" t="s" s="0">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="64">
@@ -1186,13 +1186,13 @@
         <v>63.0</v>
       </c>
       <c r="B64" t="s" s="0">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C64" t="s" s="0">
-        <v>78</v>
+        <v>40</v>
       </c>
       <c r="D64" t="s" s="0">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="65">
@@ -1200,13 +1200,13 @@
         <v>64.0</v>
       </c>
       <c r="B65" t="s" s="0">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C65" t="s" s="0">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="D65" t="s" s="0">
-        <v>41</v>
+        <v>64</v>
       </c>
     </row>
     <row r="66">
@@ -1214,13 +1214,13 @@
         <v>65.0</v>
       </c>
       <c r="B66" t="s" s="0">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="C66" t="s" s="0">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="D66" t="s" s="0">
-        <v>17</v>
+        <v>28</v>
       </c>
     </row>
     <row r="67">
@@ -1228,13 +1228,13 @@
         <v>66.0</v>
       </c>
       <c r="B67" t="s" s="0">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="C67" t="s" s="0">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D67" t="s" s="0">
-        <v>52</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>